<commit_message>
Removed the Teresa case as an example
</commit_message>
<xml_diff>
--- a/First Characters Are Same.xlsx
+++ b/First Characters Are Same.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DDD9F0-3F76-4255-8E5B-0693FE3E2FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08F6F48-051A-4F8C-84EF-2509A7634333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>I get Teresa, which makes sense to me.</t>
+  </si>
+  <si>
+    <t>Can't just use a bare function. It has to be in a lambda.</t>
+  </si>
+  <si>
+    <t>Simple mod to remove single name cases</t>
   </si>
 </sst>
 </file>
@@ -866,10 +872,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E56BDBD-5397-4DDA-AFF9-83B3CF22F939}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,6 +960,16 @@
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F8" t="e" cm="1">
+        <f t="array" ref="F8">_xlfn.LET(
+_xlpm.fx, _xlfn.LAMBDA(_xlpm.x, _xlfn.LET(_xlpm.z, LEFT(_xlfn.TEXTSPLIT(_xlpm.x," "),1),IFERROR(AND(_xlpm.z=INDEX(_xlpm.z,,1)),FALSE))),
+_xlfn._xlws.FILTER(A2:A11,_xlfn.MAP(A2:A11,_xlpm.fx(x)))
+)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -968,6 +984,26 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
+      </c>
+      <c r="F11" t="str" cm="1">
+        <f t="array" ref="F11:F13">_xlfn.LET(
+_xlpm.fx, _xlfn.LAMBDA(_xlpm.x, _xlfn.LET(_xlpm.z, LEFT(_xlfn.TEXTSPLIT(_xlpm.x," "),1),IFERROR(AND(_xlpm.z=INDEX(_xlpm.z,,1),COLUMNS(_xlpm.z)&gt;1),FALSE))),
+_xlfn._xlws.FILTER(A2:A11,_xlfn.MAP(A2:A11,_xlfn.LAMBDA(_xlpm.x,_xlpm.fx(_xlpm.x))))
+)</f>
+        <v>Donald Duck</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F12" t="str">
+        <v>Carl Cooper Camper</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F13" t="str">
+        <v>Robert Rohnson</v>
       </c>
     </row>
   </sheetData>

</xml_diff>